<commit_message>
Fresh commit with my changes
</commit_message>
<xml_diff>
--- a/File data/Data.xlsx
+++ b/File data/Data.xlsx
@@ -1,27 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Task\Task ITWORKS Education\Automation Task\course\File data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Task\Task Ejada\Automation Task\Appium\File data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7BF4287-1B93-4058-B900-774622AA6F88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5025D4C9-5CC6-4033-979B-2271C4A389C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
-    <sheet name="FormData" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t>email</t>
   </si>
@@ -29,52 +28,7 @@
     <t>pass</t>
   </si>
   <si>
-    <t>ah</t>
-  </si>
-  <si>
     <t>Expected Result</t>
-  </si>
-  <si>
-    <t>Epic sadface: Username and password do not match any user in this service</t>
-  </si>
-  <si>
-    <t>Epic sadface: Username is required</t>
-  </si>
-  <si>
-    <t>fddf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">            </t>
-  </si>
-  <si>
-    <t xml:space="preserve">        </t>
-  </si>
-  <si>
-    <t>standard_user</t>
-  </si>
-  <si>
-    <t>Epic sadface: Password is required</t>
-  </si>
-  <si>
-    <t>secret_sauce</t>
-  </si>
-  <si>
-    <t>FirstName</t>
-  </si>
-  <si>
-    <t>LastName</t>
-  </si>
-  <si>
-    <t>Postalcode</t>
-  </si>
-  <si>
-    <t>Ahmed</t>
-  </si>
-  <si>
-    <t>Khaled</t>
-  </si>
-  <si>
-    <t>17</t>
   </si>
 </sst>
 </file>
@@ -110,9 +64,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -131,9 +84,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -171,7 +124,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -277,7 +230,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -419,7 +372,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -427,16 +380,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="13" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -447,93 +401,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>11</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{629F2581-7F19-4715-B2F7-4FF5C2CA9A03}">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="9.26953125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>